<commit_message>
cs mostly working hooray
</commit_message>
<xml_diff>
--- a/double-major-optimization-main/Data/Sheets/Buckets.xlsx
+++ b/double-major-optimization-main/Data/Sheets/Buckets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferkimball/WPI-Student-Course-Optimization-23-24/double-major-optimization-main/Data/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D0142B-DD9B-7A4A-B28B-D0E78B277EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91C23C9-787D-C041-BCDA-9D019FAE5F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN_ED" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="DS_DS_BSMS" sheetId="6" r:id="rId6"/>
     <sheet name="DS_MAJOR" sheetId="7" r:id="rId7"/>
     <sheet name="CS_MAJOR" sheetId="8" r:id="rId8"/>
+    <sheet name="CS_MAJOR3" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="808">
   <si>
     <t>Bucket Key</t>
   </si>
@@ -2084,9 +2085,6 @@
     <t>Data Privacy and Ethics</t>
   </si>
   <si>
-    <t>CS_INTRO_OTHER_CORE</t>
-  </si>
-  <si>
     <t>Core CS classes</t>
   </si>
   <si>
@@ -2135,6 +2133,12 @@
     <t>CS_SOFT_ENG</t>
   </si>
   <si>
+    <t>CS_3041, CS_3431, CS_3733</t>
+  </si>
+  <si>
+    <t>['CS 3041', 'CS 3431', 'CS_3733']</t>
+  </si>
+  <si>
     <t>['CS_CORE', 'CS_DESIGN']</t>
   </si>
   <si>
@@ -2258,12 +2262,18 @@
     <t>Math Electives</t>
   </si>
   <si>
+    <t>['MA_DEPT', 'MA_1020', 'MA_1021', 'MA_1022', 'MA_1120', 'MA_4603', 'DS_4635', 'MA_4635', 'MA_1023', 'MA_1024', 'MA_1033', 'MA_1034', 'MA_2051', 'MA_2073', 'MA_2210', 'MA_2431', 'MA_3231', 'MA_3233', 'MA_3627', 'MA_3631', 'MA_4213', 'MA_4214', 'MA_4222', 'MA_4235', 'MA_4237', 'MA_4631', 'MA_4632',  'MA_2071', 'MA_2072']</t>
+  </si>
+  <si>
     <t>['CS_GEN_MATH']</t>
   </si>
   <si>
     <t>MATH_GRAD</t>
   </si>
   <si>
+    <t>['DS_502', 'MA_543', 'MA_542', 'MA_554', 'MA_540', 'MA_541']</t>
+  </si>
+  <si>
     <t>PH_DEPT</t>
   </si>
   <si>
@@ -2369,26 +2379,86 @@
     <t>['CS_SOC_IMPS']</t>
   </si>
   <si>
-    <t>['MA_DEPT', 'MA_1020', 'MA_1021', 'MA_1022', 'MA_1120', 'MA_4603', 'DS_4635', 'MA_4635', 'MA_1023', 'MA_1024', 'MA_1033', 'MA_1034', 'MA_2051', 'MA_2073', 'MA_2210', 'MA_2431', 'MA_3231', 'MA_3233', 'MA_3627', 'MA_3631', 'MA_4213', 'MA_4214', 'MA_4222', 'MA_4235', 'MA_4237', 'MA_4631', 'MA_4632',  'MA_2071', 'MA_2072']</t>
-  </si>
-  <si>
-    <t>['DS_502', 'MA_543', 'MA_542', 'MA_554', 'MA_540', 'MA_541']</t>
-  </si>
-  <si>
-    <t>['CS 3041', 'CS 3431', 'CS_3733']</t>
-  </si>
-  <si>
-    <t>CS_3041, CS_3431, CS_3733</t>
-  </si>
-  <si>
-    <t>['CS_1101', 'CS_1102', 'CS_2011', 'CS_2102', 'CS_2103', 'CS_2223', 'CS_2301', 'CS_2303', 'CS_3516']</t>
+    <t>['CS_CORE', 'CS_1000_REST']</t>
+  </si>
+  <si>
+    <t>['CS_1101', 'CS_1102']</t>
+  </si>
+  <si>
+    <t>['CS_2011', 'CS_2223', 'CS_3041', 'CS_3431', 'CS_3516']</t>
+  </si>
+  <si>
+    <t>['CS_CORE', 'CS_OBJ_OR_REST']</t>
+  </si>
+  <si>
+    <t>['CS_2102', 'CS_2103']</t>
+  </si>
+  <si>
+    <t>['CS_CORE', 'CS_SYS_REST']</t>
+  </si>
+  <si>
+    <t>['CS_2301', 'CS_2303']</t>
+  </si>
+  <si>
+    <t>['CS_3733']</t>
+  </si>
+  <si>
+    <t>['BCB_4002', 'CS_4802', 'BCB_4003', 'CS_4803', 'CS_4033', 'MA_3457', 'CS_4099', 'CS_4100', 'IMGD_4100', 'CS_4241', 'CS_4300', 'IMGD_4300', 'CS_4341', 'CS_4342', 'CS_4401', 'CS_4404', 'CS_4432', 'CS_4433', 'DS_4433', 'CS_4445', 'CS_4518', 'CS_4731', 'CS_4732', 'CS_4801', 'ECE_4802', 'CS_4804', 'BCB_502', 'CS_582', 'BCB_503', 'CS_583', 'CS_504', 'CS_513', 'CS_514', 'ECE_572', 'CS_521', 'CS_522', 'MA_510', 'CS_525', 'CS_526', 'RBE_526', 'CS_528', 'CS_529', 'ECE_581', 'CS_534', 'CS_538', 'CS_539', 'CS_540', 'CS_543', 'CS_545', 'ECE_545', 'CS_548', 'CS_549', 'RBE_549', 'CS_557', 'CS_558', 'CS_559', 'CS_563', 'CS_564', 'CS_571', 'CS_573', 'CS_577', 'ECE_577', 'CS_578', 'ECE_578', 'CS_585', 'DS_503', 'CS_586', 'DS_504', 'CS_673', 'ECE_673', 'CS_5008', 'CS_541', 'DS_541', 'CS_547', 'DS_547', 'CS_565', 'SEME_565', 'CS_566', 'SEME_566', 'CS_567', 'SEME_567', 'CS_568', 'SEME_568']</t>
+  </si>
+  <si>
+    <t>['CS_4120', 'CS_4123', 'CS_4533', 'CS_4536', 'CS_503', 'CS_536', 'CS_544', 'CS_584', 'CS_5003', 'CS_5084']</t>
+  </si>
+  <si>
+    <t>['CS_4233', 'CS_509', 'CS_542', 'CS_546', 'CS_561', 'CS_562']</t>
+  </si>
+  <si>
+    <t>['CS_4513', 'CS_4515', 'CS_4516', 'CS_502', 'CS_533', 'CS_535']</t>
+  </si>
+  <si>
+    <t>['MA_DEPT', 'MA_1020', 'MA_1021', 'MA_1022', 'MA_1120', 'MA_4603', 'DS_4635', 'MA_4635', 'MA_1023', 'MA_1024', 'MA_1033', 'MA_1034', 'MA_2051', 'MA_2073', 'MA_2210', 'MA_2431', 'MA_3231', 'MA_3233', 'MA_3627', 'MA_3631', 'MA_4213', 'MA_4214', 'MA_4222', 'MA_4235', 'MA_4237', 'MA_4631', 'MA_4632', 'DS_502', 'MA_543', 'MA_542', 'MA_554', 'MA_540', 'MA_541', 'MA_2071', 'MA_2072']</t>
+  </si>
+  <si>
+    <t>['CS_DESIGN']</t>
+  </si>
+  <si>
+    <t>['CS 3041', 'CS 3431']</t>
+  </si>
+  <si>
+    <t>['CS_OBJ_OR_REST']</t>
+  </si>
+  <si>
+    <t>['CS_210X']</t>
+  </si>
+  <si>
+    <t>CS_1101 OR CS_1102</t>
+  </si>
+  <si>
+    <t>CS_1000</t>
+  </si>
+  <si>
+    <t>CS_OOP</t>
+  </si>
+  <si>
+    <t>CS_2102 OR CS_2103</t>
+  </si>
+  <si>
+    <t>CS_SYS</t>
+  </si>
+  <si>
+    <t>CS_2301 OR CS_2303</t>
+  </si>
+  <si>
+    <t>['CS_2011', 'CS_2223', 'CS_3516']</t>
+  </si>
+  <si>
+    <t>CS_INTRO_OTHER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2441,6 +2511,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2450,7 +2526,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2529,11 +2605,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2587,6 +2678,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9252,10 +9346,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9294,10 +9388,10 @@
     </row>
     <row r="2" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>685</v>
+        <v>807</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>65</v>
@@ -9306,41 +9400,41 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>685</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>686</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>784</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>687</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>688</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="5" t="s">
         <v>689</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="18" t="s">
         <v>690</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -9352,13 +9446,13 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
+        <v>692</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>693</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="18" t="s">
         <v>694</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9381,12 +9475,12 @@
         <v>390</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -9398,41 +9492,41 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
+        <v>697</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="18" t="s">
         <v>699</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>700</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
         <v>701</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>783</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>782</v>
+        <v>702</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B8">
         <v>26</v>
@@ -9444,18 +9538,18 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B9">
         <v>57</v>
@@ -9467,18 +9561,18 @@
         <v>4.5</v>
       </c>
       <c r="E9" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -9490,18 +9584,18 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -9513,18 +9607,18 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -9536,18 +9630,18 @@
         <v>4.5</v>
       </c>
       <c r="E12" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -9559,18 +9653,18 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -9582,18 +9676,18 @@
         <v>4.5</v>
       </c>
       <c r="E14" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -9605,18 +9699,18 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -9628,18 +9722,18 @@
         <v>4.5</v>
       </c>
       <c r="E16" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -9651,13 +9745,13 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9674,18 +9768,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>554</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B19">
         <v>29</v>
@@ -9697,18 +9791,18 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>780</v>
+        <v>744</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -9720,18 +9814,18 @@
         <v>4.5</v>
       </c>
       <c r="E20" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>781</v>
+        <v>747</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -9743,18 +9837,18 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -9766,18 +9860,18 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="B23">
         <v>10</v>
@@ -9789,18 +9883,18 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -9812,18 +9906,18 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="B25">
         <v>20</v>
@@ -9835,13 +9929,13 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9849,7 +9943,7 @@
         <v>19</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <v>20</v>
@@ -9869,10 +9963,10 @@
     </row>
     <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>20</v>
@@ -9895,7 +9989,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C28">
         <v>20</v>
@@ -9918,7 +10012,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C29">
         <v>20</v>
@@ -9941,7 +10035,7 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <v>20</v>
@@ -9961,7 +10055,7 @@
     </row>
     <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -9973,18 +10067,18 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>357</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -9996,7 +10090,7 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>360</v>
@@ -10007,10 +10101,10 @@
     </row>
     <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -10030,10 +10124,10 @@
     </row>
     <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>25</v>
@@ -10076,7 +10170,7 @@
     </row>
     <row r="36" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="B36">
         <v>10</v>
@@ -10088,10 +10182,10 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>372</v>
@@ -10099,7 +10193,7 @@
     </row>
     <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -10111,18 +10205,18 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -10134,13 +10228,753 @@
         <v>3</v>
       </c>
       <c r="E38" t="s">
+        <v>780</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>801</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>101</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>800</v>
+      </c>
+      <c r="F39" t="s">
+        <v>784</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>802</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>101</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>803</v>
+      </c>
+      <c r="F40" t="s">
+        <v>787</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>804</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>85</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>805</v>
+      </c>
+      <c r="F41" t="s">
+        <v>789</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>788</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="73" customWidth="1"/>
+    <col min="7" max="7" width="36.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>784</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>785</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>689</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>787</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>789</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>693</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>390</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>698</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>790</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>83</v>
+      </c>
+      <c r="C11">
+        <v>83</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>791</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>713</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>792</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>793</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>794</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>738</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>554</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>795</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>749</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>752</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>755</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>758</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>762</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>341</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>344</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>347</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>350</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>353</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>357</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>360</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>363</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>366</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>368</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>774</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
         <v>777</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="G35" s="20" t="s">
         <v>778</v>
       </c>
-      <c r="G38" s="18" t="s">
-        <v>779</v>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="F36" t="s">
+        <v>797</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>799</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="F38" t="s">
+        <v>781</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ME up and running shockingly quickly
</commit_message>
<xml_diff>
--- a/double-major-optimization-main/Data/Sheets/Buckets.xlsx
+++ b/double-major-optimization-main/Data/Sheets/Buckets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferkimball/WPI-Student-Course-Optimization-23-24/double-major-optimization-main/Data/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91C23C9-787D-C041-BCDA-9D019FAE5F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E337C6-A488-934A-9E75-029652B1D4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN_ED" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="DS_MAJOR" sheetId="7" r:id="rId7"/>
     <sheet name="CS_MAJOR" sheetId="8" r:id="rId8"/>
     <sheet name="CS_MAJOR3" sheetId="9" r:id="rId9"/>
+    <sheet name="ME_MAJOR" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="874">
   <si>
     <t>Bucket Key</t>
   </si>
@@ -2085,9 +2086,15 @@
     <t>Data Privacy and Ethics</t>
   </si>
   <si>
+    <t>CS_INTRO_OTHER</t>
+  </si>
+  <si>
     <t>Core CS classes</t>
   </si>
   <si>
+    <t>['CS_2011', 'CS_2223', 'CS_3516']</t>
+  </si>
+  <si>
     <t>['CS_CORE']</t>
   </si>
   <si>
@@ -2379,27 +2386,45 @@
     <t>['CS_SOC_IMPS']</t>
   </si>
   <si>
+    <t>CS_1000</t>
+  </si>
+  <si>
+    <t>CS_1101 OR CS_1102</t>
+  </si>
+  <si>
+    <t>['CS_1101', 'CS_1102']</t>
+  </si>
+  <si>
     <t>['CS_CORE', 'CS_1000_REST']</t>
   </si>
   <si>
-    <t>['CS_1101', 'CS_1102']</t>
+    <t>CS_OOP</t>
+  </si>
+  <si>
+    <t>CS_2102 OR CS_2103</t>
+  </si>
+  <si>
+    <t>['CS_2102', 'CS_2103']</t>
+  </si>
+  <si>
+    <t>['CS_CORE', 'CS_OBJ_OR_REST']</t>
+  </si>
+  <si>
+    <t>CS_SYS</t>
+  </si>
+  <si>
+    <t>CS_2301 OR CS_2303</t>
+  </si>
+  <si>
+    <t>['CS_2301', 'CS_2303']</t>
+  </si>
+  <si>
+    <t>['CS_CORE', 'CS_SYS_REST']</t>
   </si>
   <si>
     <t>['CS_2011', 'CS_2223', 'CS_3041', 'CS_3431', 'CS_3516']</t>
   </si>
   <si>
-    <t>['CS_CORE', 'CS_OBJ_OR_REST']</t>
-  </si>
-  <si>
-    <t>['CS_2102', 'CS_2103']</t>
-  </si>
-  <si>
-    <t>['CS_CORE', 'CS_SYS_REST']</t>
-  </si>
-  <si>
-    <t>['CS_2301', 'CS_2303']</t>
-  </si>
-  <si>
     <t>['CS_3733']</t>
   </si>
   <si>
@@ -2418,47 +2443,221 @@
     <t>['MA_DEPT', 'MA_1020', 'MA_1021', 'MA_1022', 'MA_1120', 'MA_4603', 'DS_4635', 'MA_4635', 'MA_1023', 'MA_1024', 'MA_1033', 'MA_1034', 'MA_2051', 'MA_2073', 'MA_2210', 'MA_2431', 'MA_3231', 'MA_3233', 'MA_3627', 'MA_3631', 'MA_4213', 'MA_4214', 'MA_4222', 'MA_4235', 'MA_4237', 'MA_4631', 'MA_4632', 'DS_502', 'MA_543', 'MA_542', 'MA_554', 'MA_540', 'MA_541', 'MA_2071', 'MA_2072']</t>
   </si>
   <si>
+    <t>['CS 3041', 'CS 3431']</t>
+  </si>
+  <si>
     <t>['CS_DESIGN']</t>
   </si>
   <si>
-    <t>['CS 3041', 'CS 3431']</t>
+    <t>['CS_210X']</t>
   </si>
   <si>
     <t>['CS_OBJ_OR_REST']</t>
   </si>
   <si>
-    <t>['CS_210X']</t>
-  </si>
-  <si>
-    <t>CS_1101 OR CS_1102</t>
-  </si>
-  <si>
-    <t>CS_1000</t>
-  </si>
-  <si>
-    <t>CS_OOP</t>
-  </si>
-  <si>
-    <t>CS_2102 OR CS_2103</t>
-  </si>
-  <si>
-    <t>CS_SYS</t>
-  </si>
-  <si>
-    <t>CS_2301 OR CS_2303</t>
-  </si>
-  <si>
-    <t>['CS_2011', 'CS_2223', 'CS_3516']</t>
-  </si>
-  <si>
-    <t>CS_INTRO_OTHER</t>
+    <t>['ECON_DEPT', 'ENV_DEPT', 'GOV_DEPT', 'PSY_DEPT', 'SD_DEPT', 'SOC_DEPT', 'SS_DEPT', 'STS_DEPT', 'DEV_DEPT', 'GOV_2314', 'GOV_2315', 'GOV_2313']</t>
+  </si>
+  <si>
+    <t>['ME_BSCAP', 'ME_CHEM']</t>
+  </si>
+  <si>
+    <t>['CH_1010', 'CH_1020']</t>
+  </si>
+  <si>
+    <t>['ME_BSCAP', 'ME_PHY']</t>
+  </si>
+  <si>
+    <t>['PH_1110', 'PH_1120', 'PH_1111', 'PH_1121']</t>
+  </si>
+  <si>
+    <t>['ME_BSCAP', 'ME_MABS', 'ME_PHY']</t>
+  </si>
+  <si>
+    <t>['PH_2101']</t>
+  </si>
+  <si>
+    <t>['ME_BSCAP', 'ME_MABS', 'ME_CHEM', 'ME_ES_3001_EQ']</t>
+  </si>
+  <si>
+    <t>['CH_3510']</t>
+  </si>
+  <si>
+    <t>['ME_M']</t>
+  </si>
+  <si>
+    <t>['MA_1021', 'MA_1022', 'MA_1023', 'MA_1024', 'MA_2071', 'MA_2051']</t>
+  </si>
+  <si>
+    <t>['ME_MABS']</t>
+  </si>
+  <si>
+    <t>['MA_DEPT', 'CH_DEPT', 'PH_DEPT', 'GE_DEPT', 'BB_DEPT']</t>
+  </si>
+  <si>
+    <t>['ME_MS', 'ME_MS_CORE']</t>
+  </si>
+  <si>
+    <t>['ES_2501', 'ES_2502', 'ES_2503']</t>
+  </si>
+  <si>
+    <t>['ME_MS']</t>
+  </si>
+  <si>
+    <t>['ME_4320', 'ME_4322', 'ME_4323', 'ME_4324', 'RBE_4322']</t>
+  </si>
+  <si>
+    <t>['ME_TS', 'ME_TS_CORE']</t>
+  </si>
+  <si>
+    <t>['ES_3003', 'ES_3004']</t>
+  </si>
+  <si>
+    <t>['ME_TS']</t>
+  </si>
+  <si>
+    <t>['ME_4422', 'ME_4429']</t>
+  </si>
+  <si>
+    <t>['ME_MAT_SCI']</t>
+  </si>
+  <si>
+    <t>['ES_2001']</t>
+  </si>
+  <si>
+    <t>['ME_ECE', 'ME_E']</t>
+  </si>
+  <si>
+    <t>['ME_EXP']</t>
+  </si>
+  <si>
+    <t>['ME_3901', 'ME_3902']</t>
+  </si>
+  <si>
+    <t>['ME_PROG']</t>
+  </si>
+  <si>
+    <t>['ME_2312', 'ME_4512', 'BME_1004', 'CS_1101', 'CS_1004']</t>
+  </si>
+  <si>
+    <t>['ME_E', 'ME_ES_3001_EQ']</t>
+  </si>
+  <si>
+    <t>['ES_3001']</t>
+  </si>
+  <si>
+    <t>['ME_E']</t>
+  </si>
+  <si>
+    <t>['ES_DEPT', 'ME_DEPT', 'AREN_DEPT', 'CHE_DEPT', 'RBE_DEPT', 'CE_DEPT', 'AE_DEPT', 'OIE_DEPT', 'FP_DEPT']</t>
+  </si>
+  <si>
+    <t>['ME_OTHER_ECE']</t>
+  </si>
+  <si>
+    <t>['ECE_1799']</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>PH_2101</t>
+  </si>
+  <si>
+    <t>CH_3510</t>
+  </si>
+  <si>
+    <t>Math Core</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math or Basic Science </t>
+  </si>
+  <si>
+    <t>Mechanical Systems Core</t>
+  </si>
+  <si>
+    <t>ME_4320, ME_4322, RBE_4322, ME_4323, ME_4324</t>
+  </si>
+  <si>
+    <t>Thermofluid Systems Core</t>
+  </si>
+  <si>
+    <t>ME_4222 OR ME_4429</t>
+  </si>
+  <si>
+    <t>ES_2001</t>
+  </si>
+  <si>
+    <t>['ECE_DEPT', 'ECE_2010']</t>
+  </si>
+  <si>
+    <t>ECE classes</t>
+  </si>
+  <si>
+    <t>ME_3901 OR ME_3902</t>
+  </si>
+  <si>
+    <t>BME_1004, CS_1004, CS_1101, ME_2312, ME_4512</t>
+  </si>
+  <si>
+    <t>ES_3001</t>
+  </si>
+  <si>
+    <t>CHEM</t>
+  </si>
+  <si>
+    <t>PHYS</t>
+  </si>
+  <si>
+    <t>CHEM_THERMO</t>
+  </si>
+  <si>
+    <t>PH_THERMO</t>
+  </si>
+  <si>
+    <t>MABS</t>
+  </si>
+  <si>
+    <t>MECH_SYS_CORE</t>
+  </si>
+  <si>
+    <t>MECH_SYS_4000</t>
+  </si>
+  <si>
+    <t>THERMO_CORE</t>
+  </si>
+  <si>
+    <t>THERMO_4000</t>
+  </si>
+  <si>
+    <t>MAT_SCI</t>
+  </si>
+  <si>
+    <t>ECE</t>
+  </si>
+  <si>
+    <t>ME_EXP</t>
+  </si>
+  <si>
+    <t>PROG</t>
+  </si>
+  <si>
+    <t>THERMO_INTRO</t>
+  </si>
+  <si>
+    <t>ECE_NOT</t>
+  </si>
+  <si>
+    <t>HOW DID THIS SHOW UP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2517,6 +2716,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2526,7 +2731,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2620,11 +2825,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2681,6 +2901,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3274,6 +3500,671 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="43" style="5" customWidth="1"/>
+    <col min="7" max="7" width="32.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>766</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>770</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>771</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>772</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>773</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>774</v>
+      </c>
+      <c r="B11">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>775</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>858</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>842</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>859</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>843</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>812</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>861</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>844</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>860</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>845</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>675</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>846</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>818</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>862</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>847</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>863</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>848</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>822</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>864</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>849</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>824</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>865</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>850</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>826</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>866</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>851</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>867</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>852</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>868</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>854</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>869</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>855</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>870</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>856</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>871</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>80</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>857</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>837</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>762</v>
+      </c>
+      <c r="B27">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>763</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>872</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>873</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>840</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G27"/>
@@ -9348,7 +10239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="116" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -9388,7 +10279,7 @@
     </row>
     <row r="2" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>807</v>
+        <v>685</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -9400,18 +10291,18 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>806</v>
+        <v>687</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -9423,18 +10314,18 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -9446,13 +10337,13 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9475,12 +10366,12 @@
         <v>390</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -9492,18 +10383,18 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -9515,18 +10406,18 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B8">
         <v>26</v>
@@ -9538,18 +10429,18 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B9">
         <v>57</v>
@@ -9561,18 +10452,18 @@
         <v>4.5</v>
       </c>
       <c r="E9" t="s">
+        <v>711</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>709</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>710</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -9584,18 +10475,18 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -9607,18 +10498,18 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -9630,18 +10521,18 @@
         <v>4.5</v>
       </c>
       <c r="E12" t="s">
+        <v>722</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="G12" s="18" t="s">
         <v>720</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -9653,18 +10544,18 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -9676,18 +10567,18 @@
         <v>4.5</v>
       </c>
       <c r="E14" t="s">
+        <v>729</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G14" s="18" t="s">
         <v>727</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>728</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -9699,18 +10590,18 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -9722,18 +10613,18 @@
         <v>4.5</v>
       </c>
       <c r="E16" t="s">
+        <v>736</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="G16" s="18" t="s">
         <v>734</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -9745,13 +10636,13 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9768,18 +10659,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>554</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B19">
         <v>29</v>
@@ -9791,18 +10682,18 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -9814,18 +10705,18 @@
         <v>4.5</v>
       </c>
       <c r="E20" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="F20" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="G20" s="18" t="s">
         <v>747</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -9837,18 +10728,18 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -9860,18 +10751,18 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="B23">
         <v>10</v>
@@ -9883,18 +10774,18 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -9906,18 +10797,18 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="B25">
         <v>20</v>
@@ -9929,13 +10820,13 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9963,7 +10854,7 @@
     </row>
     <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -10055,7 +10946,7 @@
     </row>
     <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -10067,18 +10958,18 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>357</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -10090,7 +10981,7 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>360</v>
@@ -10101,7 +10992,7 @@
     </row>
     <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -10124,7 +11015,7 @@
     </row>
     <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -10170,7 +11061,7 @@
     </row>
     <row r="36" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="B36">
         <v>10</v>
@@ -10182,10 +11073,10 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>372</v>
@@ -10193,7 +11084,7 @@
     </row>
     <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -10205,18 +11096,18 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -10228,18 +11119,18 @@
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>801</v>
+        <v>785</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -10251,18 +11142,18 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>800</v>
+        <v>786</v>
       </c>
       <c r="F39" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>783</v>
+        <v>788</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>802</v>
+        <v>789</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -10274,18 +11165,18 @@
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>803</v>
+        <v>790</v>
       </c>
       <c r="F40" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>786</v>
+        <v>792</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>804</v>
+        <v>793</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -10297,13 +11188,13 @@
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>805</v>
+        <v>794</v>
       </c>
       <c r="F41" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>788</v>
+        <v>796</v>
       </c>
     </row>
   </sheetData>
@@ -10359,10 +11250,10 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>783</v>
+        <v>788</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -10376,10 +11267,10 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -10393,10 +11284,10 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -10410,10 +11301,10 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>786</v>
+        <v>792</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -10427,10 +11318,10 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>788</v>
+        <v>796</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -10444,10 +11335,10 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -10464,7 +11355,7 @@
         <v>390</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -10478,10 +11369,10 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -10495,10 +11386,10 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>790</v>
+        <v>798</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -10512,10 +11403,10 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>791</v>
+        <v>799</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -10529,10 +11420,10 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -10546,10 +11437,10 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>792</v>
+        <v>800</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -10563,10 +11454,10 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>793</v>
+        <v>801</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -10580,10 +11471,10 @@
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>794</v>
+        <v>802</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -10597,10 +11488,10 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
@@ -10617,7 +11508,7 @@
         <v>554</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
@@ -10631,10 +11522,10 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>795</v>
+        <v>803</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -10648,10 +11539,10 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
@@ -10665,10 +11556,10 @@
         <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
@@ -10682,10 +11573,10 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
@@ -10699,10 +11590,10 @@
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -10716,10 +11607,10 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -10821,7 +11712,7 @@
         <v>357</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -10903,7 +11794,7 @@
         <v>3</v>
       </c>
       <c r="F34" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>372</v>
@@ -10920,10 +11811,10 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -10937,10 +11828,10 @@
         <v>3</v>
       </c>
       <c r="F36" t="s">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -10954,10 +11845,10 @@
         <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>798</v>
+        <v>807</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -10971,10 +11862,10 @@
         <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to debug orig_credits_used
</commit_message>
<xml_diff>
--- a/double-major-optimization-main/Data/Sheets/Buckets.xlsx
+++ b/double-major-optimization-main/Data/Sheets/Buckets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferkimball/WPI-Student-Course-Optimization-23-24/double-major-optimization-main/Data/Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wpi0-my.sharepoint.com/personal/mrsuyer_wpi_edu/Documents/MQP/WPI-Student-Course-Optimization-23-24/double-major-optimization-main/Data/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91C23C9-787D-C041-BCDA-9D019FAE5F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{E91C23C9-787D-C041-BCDA-9D019FAE5F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EB176A1-18C9-410C-A6F0-F261A6754D24}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN_ED" sheetId="1" r:id="rId1"/>
@@ -3002,19 +3002,19 @@
       <selection activeCell="A2" sqref="A2:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="5" customWidth="1"/>
-    <col min="3" max="4" width="13.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="39.1640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="36.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="26.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="5" customWidth="1"/>
+    <col min="3" max="4" width="13.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="39.109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="26.44140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3038,7 +3038,7 @@
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="58.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -3282,16 +3282,16 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="58.5" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="58.44140625" customWidth="1"/>
     <col min="7" max="7" width="70.6640625" customWidth="1"/>
-    <col min="8" max="8" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>63</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>67</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>71</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>75</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>79</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>83</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>87</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>95</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
     </row>
   </sheetData>
@@ -3906,18 +3906,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="5" customWidth="1"/>
-    <col min="3" max="5" width="13.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="31.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="71.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="5" customWidth="1"/>
+    <col min="3" max="5" width="13.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="71.44140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="32" style="5" customWidth="1"/>
-    <col min="9" max="9" width="39.5" style="5" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="58.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>105</v>
       </c>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>109</v>
       </c>
@@ -4014,7 +4014,7 @@
       </c>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>113</v>
       </c>
@@ -4038,7 +4038,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>117</v>
       </c>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>121</v>
       </c>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>125</v>
       </c>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>129</v>
       </c>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="44.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="44.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>133</v>
       </c>
@@ -4158,7 +4158,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>137</v>
       </c>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>141</v>
       </c>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>145</v>
       </c>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="58.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>149</v>
       </c>
@@ -4254,7 +4254,7 @@
       </c>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="58.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>153</v>
       </c>
@@ -4278,7 +4278,7 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>157</v>
       </c>
@@ -4302,7 +4302,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>161</v>
       </c>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>165</v>
       </c>
@@ -4350,7 +4350,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>169</v>
       </c>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>172</v>
       </c>
@@ -4398,7 +4398,7 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>176</v>
       </c>
@@ -4422,7 +4422,7 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" ht="72.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="72.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>180</v>
       </c>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>183</v>
       </c>
@@ -4470,7 +4470,7 @@
       </c>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>187</v>
       </c>
@@ -4494,7 +4494,7 @@
       </c>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>190</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>194</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>198</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>23</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="72.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="72.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -4803,22 +4803,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="5" customWidth="1"/>
-    <col min="3" max="5" width="13.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="54.1640625" style="10" customWidth="1"/>
+    <col min="3" max="5" width="13.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="54.109375" style="10" customWidth="1"/>
     <col min="7" max="7" width="63.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="38.5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.5" customWidth="1"/>
+    <col min="8" max="8" width="38.44140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4842,7 +4842,7 @@
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>105</v>
       </c>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -4914,7 +4914,7 @@
       </c>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -4938,7 +4938,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
@@ -4962,7 +4962,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>109</v>
       </c>
@@ -5010,7 +5010,7 @@
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>113</v>
       </c>
@@ -5034,7 +5034,7 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>117</v>
       </c>
@@ -5058,7 +5058,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>121</v>
       </c>
@@ -5082,7 +5082,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>215</v>
       </c>
@@ -5106,7 +5106,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>67</v>
       </c>
@@ -5130,7 +5130,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>125</v>
       </c>
@@ -5154,7 +5154,7 @@
       </c>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>129</v>
       </c>
@@ -5178,7 +5178,7 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>133</v>
       </c>
@@ -5202,7 +5202,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>227</v>
       </c>
@@ -5226,7 +5226,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>63</v>
       </c>
@@ -5250,7 +5250,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>234</v>
       </c>
@@ -5274,7 +5274,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>236</v>
       </c>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>79</v>
       </c>
@@ -5346,7 +5346,7 @@
       </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>83</v>
       </c>
@@ -5370,7 +5370,7 @@
       </c>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>149</v>
       </c>
@@ -5394,15 +5394,15 @@
       </c>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>244</v>
       </c>
       <c r="B25" s="3">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C25" s="3">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D25" s="3">
         <v>3</v>
@@ -5418,15 +5418,15 @@
       </c>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="3">
         <v>3</v>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>153</v>
       </c>
@@ -5466,7 +5466,7 @@
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>157</v>
       </c>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>161</v>
       </c>
@@ -5514,7 +5514,7 @@
       </c>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>165</v>
       </c>
@@ -5538,7 +5538,7 @@
       </c>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>198</v>
       </c>
@@ -5562,7 +5562,7 @@
       </c>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>183</v>
       </c>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>91</v>
       </c>
@@ -5610,7 +5610,7 @@
       </c>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>194</v>
       </c>
@@ -5634,7 +5634,7 @@
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>187</v>
       </c>
@@ -5658,7 +5658,7 @@
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>262</v>
       </c>
@@ -5682,7 +5682,7 @@
       </c>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>176</v>
       </c>
@@ -5706,7 +5706,7 @@
       </c>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>172</v>
       </c>
@@ -5730,7 +5730,7 @@
       </c>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>190</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>267</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>95</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>99</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>169</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>180</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>7</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>15</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>19</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>26</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>29</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>32</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>35</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>39</v>
       </c>
@@ -6112,17 +6112,17 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="48.5" customWidth="1"/>
+    <col min="6" max="6" width="48.44140625" customWidth="1"/>
     <col min="7" max="7" width="71.6640625" customWidth="1"/>
-    <col min="8" max="8" width="51.5" customWidth="1"/>
+    <col min="8" max="8" width="51.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>276</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>280</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>284</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>288</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>292</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>296</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>300</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>304</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>308</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>312</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>316</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>320</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>324</v>
       </c>
@@ -6444,7 +6444,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>328</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>332</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>336</v>
       </c>
@@ -6526,15 +6526,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" customWidth="1"/>
     <col min="6" max="6" width="49" customWidth="1"/>
-    <col min="7" max="7" width="60.5" customWidth="1"/>
+    <col min="7" max="7" width="60.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -6603,7 +6603,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -6649,7 +6649,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -6672,7 +6672,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>355</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -6764,7 +6764,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>373</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>377</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>381</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>385</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>389</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>392</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>396</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>400</v>
       </c>
@@ -6994,7 +6994,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>404</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>408</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>412</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>416</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>420</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>424</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>428</v>
       </c>
@@ -7155,7 +7155,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>432</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>436</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>440</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>444</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>448</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>452</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>456</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>460</v>
       </c>
@@ -7339,7 +7339,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>464</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>468</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>472</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>476</v>
       </c>
@@ -7431,7 +7431,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>480</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>484</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>488</v>
       </c>
@@ -7500,7 +7500,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>492</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>496</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>500</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>504</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>507</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>510</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>514</v>
       </c>
@@ -7661,7 +7661,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>518</v>
       </c>
@@ -7684,7 +7684,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>521</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>525</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>528</v>
       </c>
@@ -7753,7 +7753,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>532</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>536</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>540</v>
       </c>
@@ -7822,7 +7822,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>544</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>548</v>
       </c>
@@ -7868,7 +7868,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>552</v>
       </c>
@@ -7891,7 +7891,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>556</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>560</v>
       </c>
@@ -7937,7 +7937,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>564</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>568</v>
       </c>
@@ -7983,7 +7983,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>572</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>576</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>580</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>584</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>587</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>591</v>
       </c>
@@ -8121,7 +8121,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>593</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>595</v>
       </c>
@@ -8167,7 +8167,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>599</v>
       </c>
@@ -8190,7 +8190,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>603</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>607</v>
       </c>
@@ -8236,7 +8236,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>609</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>611</v>
       </c>
@@ -8282,7 +8282,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>615</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>619</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>623</v>
       </c>
@@ -8364,15 +8364,15 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="44.83203125" customWidth="1"/>
-    <col min="6" max="6" width="46.5" customWidth="1"/>
-    <col min="7" max="7" width="45.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="44.77734375" customWidth="1"/>
+    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="7" max="7" width="45.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -8418,7 +8418,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -8441,7 +8441,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -8464,7 +8464,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -8487,7 +8487,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -8510,7 +8510,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>627</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -8556,7 +8556,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -8603,7 +8603,7 @@
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -8626,7 +8626,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -8649,7 +8649,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>628</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>377</v>
       </c>
@@ -8695,7 +8695,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>630</v>
       </c>
@@ -8718,7 +8718,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>632</v>
       </c>
@@ -8741,7 +8741,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>634</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>635</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>637</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>640</v>
       </c>
@@ -8833,7 +8833,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>643</v>
       </c>
@@ -8856,7 +8856,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>647</v>
       </c>
@@ -8879,7 +8879,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>649</v>
       </c>
@@ -8902,7 +8902,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>653</v>
       </c>
@@ -8925,7 +8925,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>655</v>
       </c>
@@ -8948,7 +8948,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>658</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>661</v>
       </c>
@@ -8994,7 +8994,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>664</v>
       </c>
@@ -9017,7 +9017,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>667</v>
       </c>
@@ -9040,7 +9040,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>460</v>
       </c>
@@ -9063,7 +9063,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>668</v>
       </c>
@@ -9086,7 +9086,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>672</v>
       </c>
@@ -9109,7 +9109,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>675</v>
       </c>
@@ -9132,7 +9132,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>677</v>
       </c>
@@ -9155,7 +9155,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>548</v>
       </c>
@@ -9178,7 +9178,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>679</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>556</v>
       </c>
@@ -9224,7 +9224,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>560</v>
       </c>
@@ -9247,7 +9247,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>680</v>
       </c>
@@ -9270,7 +9270,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>682</v>
       </c>
@@ -9293,7 +9293,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>572</v>
       </c>
@@ -9316,7 +9316,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>683</v>
       </c>
@@ -9348,22 +9348,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+    <sheetView zoomScale="116" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="72.83203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="72.77734375" style="5" customWidth="1"/>
     <col min="7" max="7" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -9386,7 +9386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>807</v>
       </c>
@@ -9409,7 +9409,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>687</v>
       </c>
@@ -9432,7 +9432,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>691</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>389</v>
       </c>
@@ -9478,7 +9478,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>696</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>700</v>
       </c>
@@ -9524,7 +9524,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="64.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>704</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>708</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>711</v>
       </c>
@@ -9593,7 +9593,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>715</v>
       </c>
@@ -9616,7 +9616,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>719</v>
       </c>
@@ -9639,7 +9639,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>722</v>
       </c>
@@ -9662,7 +9662,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>726</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>729</v>
       </c>
@@ -9708,7 +9708,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>733</v>
       </c>
@@ -9731,7 +9731,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>736</v>
       </c>
@@ -9754,7 +9754,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>552</v>
       </c>
@@ -9777,7 +9777,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="64.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>742</v>
       </c>
@@ -9800,7 +9800,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>746</v>
       </c>
@@ -9823,7 +9823,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>748</v>
       </c>
@@ -9846,7 +9846,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>751</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>754</v>
       </c>
@@ -9892,7 +9892,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>757</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>760</v>
       </c>
@@ -9938,7 +9938,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>764</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -10007,7 +10007,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -10030,7 +10030,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -10053,7 +10053,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>765</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>768</v>
       </c>
@@ -10099,7 +10099,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>770</v>
       </c>
@@ -10122,7 +10122,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>771</v>
       </c>
@@ -10145,7 +10145,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -10168,7 +10168,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>772</v>
       </c>
@@ -10191,7 +10191,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>775</v>
       </c>
@@ -10214,7 +10214,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>779</v>
       </c>
@@ -10237,7 +10237,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>801</v>
       </c>
@@ -10260,7 +10260,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>802</v>
       </c>
@@ -10283,7 +10283,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>804</v>
       </c>
@@ -10319,13 +10319,13 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="73" customWidth="1"/>
-    <col min="7" max="7" width="36.83203125" customWidth="1"/>
+    <col min="7" max="7" width="36.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>2</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>5</v>
       </c>
@@ -10382,7 +10382,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -10399,7 +10399,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -10416,7 +10416,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -10450,7 +10450,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1</v>
       </c>
@@ -10467,7 +10467,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1</v>
       </c>
@@ -10484,7 +10484,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1</v>
       </c>
@@ -10501,7 +10501,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>83</v>
       </c>
@@ -10518,7 +10518,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>2</v>
       </c>
@@ -10535,7 +10535,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>
@@ -10552,7 +10552,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>6</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>6</v>
       </c>
@@ -10586,7 +10586,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>2</v>
       </c>
@@ -10603,7 +10603,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>2</v>
       </c>
@@ -10620,7 +10620,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>35</v>
       </c>
@@ -10637,7 +10637,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>1</v>
       </c>
@@ -10654,7 +10654,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>1</v>
       </c>
@@ -10671,7 +10671,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>1</v>
       </c>
@@ -10688,7 +10688,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>1</v>
       </c>
@@ -10705,7 +10705,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>7</v>
       </c>
@@ -10722,7 +10722,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>3</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>4</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>2</v>
       </c>
@@ -10773,7 +10773,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>3</v>
       </c>
@@ -10790,7 +10790,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>2</v>
       </c>
@@ -10807,7 +10807,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>3</v>
       </c>
@@ -10824,7 +10824,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>2</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>5</v>
       </c>
@@ -10858,7 +10858,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>1</v>
       </c>
@@ -10875,7 +10875,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>1</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>10</v>
       </c>
@@ -10909,7 +10909,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>2</v>
       </c>
@@ -10926,7 +10926,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>2</v>
       </c>
@@ -10943,7 +10943,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>1</v>
       </c>
@@ -10960,7 +10960,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
changed process_workday.py to work with different academic progress layouts
</commit_message>
<xml_diff>
--- a/double-major-optimization-main/Data/Sheets/Buckets.xlsx
+++ b/double-major-optimization-main/Data/Sheets/Buckets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferkimball/WPI-Student-Course-Optimization-23-24/double-major-optimization-main/Data/Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wpi0-my.sharepoint.com/personal/mrsuyer_wpi_edu/Documents/MQP/WPI-Student-Course-Optimization-23-24/double-major-optimization-main/Data/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E337C6-A488-934A-9E75-029652B1D4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{88E337C6-A488-934A-9E75-029652B1D4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26F69C0F-BB23-438D-AE0B-AC4AE6D3404B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN_ED" sheetId="1" r:id="rId1"/>
@@ -3228,19 +3228,19 @@
       <selection activeCell="A2" sqref="A2:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="5" customWidth="1"/>
-    <col min="3" max="4" width="13.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="39.1640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="36.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="26.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="5" customWidth="1"/>
+    <col min="3" max="4" width="13.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="39.109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="26.44140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="58.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -3504,19 +3504,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="43" style="5" customWidth="1"/>
-    <col min="7" max="7" width="32.5" customWidth="1"/>
+    <col min="7" max="7" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>766</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>770</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>772</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>773</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>774</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>858</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>859</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>861</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>860</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>675</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>862</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>863</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>864</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>865</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>866</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>867</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>868</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>869</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>870</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>871</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>762</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>872</v>
       </c>
@@ -4173,16 +4173,16 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="58.5" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="58.44140625" customWidth="1"/>
     <col min="7" max="7" width="70.6640625" customWidth="1"/>
-    <col min="8" max="8" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>63</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>67</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>71</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>75</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>79</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>83</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>87</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>95</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
     </row>
   </sheetData>
@@ -4797,18 +4797,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="5" customWidth="1"/>
-    <col min="3" max="5" width="13.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="31.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="71.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="5" customWidth="1"/>
+    <col min="3" max="5" width="13.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="71.44140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="32" style="5" customWidth="1"/>
-    <col min="9" max="9" width="39.5" style="5" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4833,7 +4833,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -4857,7 +4857,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="58.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>105</v>
       </c>
@@ -4881,7 +4881,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>109</v>
       </c>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>113</v>
       </c>
@@ -4929,7 +4929,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>117</v>
       </c>
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>121</v>
       </c>
@@ -4977,7 +4977,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>125</v>
       </c>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>129</v>
       </c>
@@ -5025,7 +5025,7 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="44.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="44.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>133</v>
       </c>
@@ -5049,7 +5049,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>137</v>
       </c>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>141</v>
       </c>
@@ -5097,7 +5097,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>145</v>
       </c>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="58.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>149</v>
       </c>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="58.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>153</v>
       </c>
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>157</v>
       </c>
@@ -5193,7 +5193,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>161</v>
       </c>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>165</v>
       </c>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>169</v>
       </c>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>172</v>
       </c>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>176</v>
       </c>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" ht="72.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="72.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>180</v>
       </c>
@@ -5337,7 +5337,7 @@
       </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>183</v>
       </c>
@@ -5361,7 +5361,7 @@
       </c>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>187</v>
       </c>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>190</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>194</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>198</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>23</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="72.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="72.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -5694,22 +5694,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="5" customWidth="1"/>
-    <col min="3" max="5" width="13.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="54.1640625" style="10" customWidth="1"/>
+    <col min="3" max="5" width="13.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="54.109375" style="10" customWidth="1"/>
     <col min="7" max="7" width="63.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="38.5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.5" customWidth="1"/>
+    <col min="8" max="8" width="38.44140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -5733,7 +5733,7 @@
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>105</v>
       </c>
@@ -5781,7 +5781,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -5805,7 +5805,7 @@
       </c>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
@@ -5877,7 +5877,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>109</v>
       </c>
@@ -5901,7 +5901,7 @@
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>113</v>
       </c>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>117</v>
       </c>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>121</v>
       </c>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>215</v>
       </c>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>67</v>
       </c>
@@ -6021,7 +6021,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>125</v>
       </c>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>129</v>
       </c>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>133</v>
       </c>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>227</v>
       </c>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>63</v>
       </c>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>234</v>
       </c>
@@ -6165,7 +6165,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>236</v>
       </c>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
@@ -6213,7 +6213,7 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>79</v>
       </c>
@@ -6237,7 +6237,7 @@
       </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>83</v>
       </c>
@@ -6261,7 +6261,7 @@
       </c>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>149</v>
       </c>
@@ -6285,15 +6285,15 @@
       </c>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>244</v>
       </c>
       <c r="B25" s="3">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C25" s="3">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D25" s="3">
         <v>3</v>
@@ -6309,15 +6309,15 @@
       </c>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="3">
         <v>3</v>
@@ -6333,7 +6333,7 @@
       </c>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>153</v>
       </c>
@@ -6357,7 +6357,7 @@
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>157</v>
       </c>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>161</v>
       </c>
@@ -6405,7 +6405,7 @@
       </c>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>165</v>
       </c>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>198</v>
       </c>
@@ -6453,7 +6453,7 @@
       </c>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>183</v>
       </c>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>91</v>
       </c>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>194</v>
       </c>
@@ -6525,7 +6525,7 @@
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>187</v>
       </c>
@@ -6549,7 +6549,7 @@
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>262</v>
       </c>
@@ -6573,7 +6573,7 @@
       </c>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>176</v>
       </c>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>172</v>
       </c>
@@ -6621,7 +6621,7 @@
       </c>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>190</v>
       </c>
@@ -6644,7 +6644,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>267</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>95</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>99</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>169</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>180</v>
       </c>
@@ -6759,7 +6759,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>7</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>15</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>19</v>
       </c>
@@ -6851,7 +6851,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>26</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>29</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>32</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>35</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>39</v>
       </c>
@@ -7003,17 +7003,17 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="48.5" customWidth="1"/>
+    <col min="6" max="6" width="48.44140625" customWidth="1"/>
     <col min="7" max="7" width="71.6640625" customWidth="1"/>
-    <col min="8" max="8" width="51.5" customWidth="1"/>
+    <col min="8" max="8" width="51.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>276</v>
       </c>
@@ -7059,7 +7059,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>280</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>284</v>
       </c>
@@ -7105,7 +7105,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>288</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>292</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>296</v>
       </c>
@@ -7174,7 +7174,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>300</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>304</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>308</v>
       </c>
@@ -7243,7 +7243,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>312</v>
       </c>
@@ -7266,7 +7266,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>316</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>320</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>324</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>328</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>332</v>
       </c>
@@ -7381,7 +7381,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>336</v>
       </c>
@@ -7417,15 +7417,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" customWidth="1"/>
     <col min="6" max="6" width="49" customWidth="1"/>
-    <col min="7" max="7" width="60.5" customWidth="1"/>
+    <col min="7" max="7" width="60.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -7471,7 +7471,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -7517,7 +7517,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>355</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -7609,7 +7609,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>373</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>377</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>381</v>
       </c>
@@ -7770,7 +7770,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>385</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>389</v>
       </c>
@@ -7816,7 +7816,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>392</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>396</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>400</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>404</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>408</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>412</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>416</v>
       </c>
@@ -7977,7 +7977,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>420</v>
       </c>
@@ -8000,7 +8000,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>424</v>
       </c>
@@ -8023,7 +8023,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>428</v>
       </c>
@@ -8046,7 +8046,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>432</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>436</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>440</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>444</v>
       </c>
@@ -8138,7 +8138,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>448</v>
       </c>
@@ -8161,7 +8161,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>452</v>
       </c>
@@ -8184,7 +8184,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>456</v>
       </c>
@@ -8207,7 +8207,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>460</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>464</v>
       </c>
@@ -8253,7 +8253,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>468</v>
       </c>
@@ -8276,7 +8276,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>472</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>476</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>480</v>
       </c>
@@ -8345,7 +8345,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>484</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>488</v>
       </c>
@@ -8391,7 +8391,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>492</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>496</v>
       </c>
@@ -8437,7 +8437,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>500</v>
       </c>
@@ -8460,7 +8460,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>504</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>507</v>
       </c>
@@ -8506,7 +8506,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>510</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>514</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>518</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>521</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>525</v>
       </c>
@@ -8621,7 +8621,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>528</v>
       </c>
@@ -8644,7 +8644,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>532</v>
       </c>
@@ -8667,7 +8667,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>536</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>540</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>544</v>
       </c>
@@ -8736,7 +8736,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>548</v>
       </c>
@@ -8759,7 +8759,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>552</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>556</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>560</v>
       </c>
@@ -8828,7 +8828,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>564</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>568</v>
       </c>
@@ -8874,7 +8874,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>572</v>
       </c>
@@ -8897,7 +8897,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>576</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>580</v>
       </c>
@@ -8943,7 +8943,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>584</v>
       </c>
@@ -8966,7 +8966,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>587</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>591</v>
       </c>
@@ -9012,7 +9012,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>593</v>
       </c>
@@ -9035,7 +9035,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>595</v>
       </c>
@@ -9058,7 +9058,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>599</v>
       </c>
@@ -9081,7 +9081,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>603</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>607</v>
       </c>
@@ -9127,7 +9127,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>609</v>
       </c>
@@ -9150,7 +9150,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>611</v>
       </c>
@@ -9173,7 +9173,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>615</v>
       </c>
@@ -9196,7 +9196,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>619</v>
       </c>
@@ -9219,7 +9219,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>623</v>
       </c>
@@ -9255,15 +9255,15 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="44.83203125" customWidth="1"/>
-    <col min="6" max="6" width="46.5" customWidth="1"/>
-    <col min="7" max="7" width="45.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="44.77734375" customWidth="1"/>
+    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="7" max="7" width="45.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -9286,7 +9286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -9332,7 +9332,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -9378,7 +9378,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -9401,7 +9401,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>627</v>
       </c>
@@ -9424,7 +9424,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -9470,7 +9470,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -9494,7 +9494,7 @@
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -9517,7 +9517,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -9540,7 +9540,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>628</v>
       </c>
@@ -9563,7 +9563,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>377</v>
       </c>
@@ -9586,7 +9586,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>630</v>
       </c>
@@ -9609,7 +9609,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>632</v>
       </c>
@@ -9632,7 +9632,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>634</v>
       </c>
@@ -9655,7 +9655,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>635</v>
       </c>
@@ -9678,7 +9678,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>637</v>
       </c>
@@ -9701,7 +9701,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>640</v>
       </c>
@@ -9724,7 +9724,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>643</v>
       </c>
@@ -9747,7 +9747,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>647</v>
       </c>
@@ -9770,7 +9770,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>649</v>
       </c>
@@ -9793,7 +9793,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>653</v>
       </c>
@@ -9816,7 +9816,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>655</v>
       </c>
@@ -9839,7 +9839,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>658</v>
       </c>
@@ -9862,7 +9862,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>661</v>
       </c>
@@ -9885,7 +9885,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>664</v>
       </c>
@@ -9908,7 +9908,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>667</v>
       </c>
@@ -9931,7 +9931,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>460</v>
       </c>
@@ -9954,7 +9954,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>668</v>
       </c>
@@ -9977,7 +9977,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>672</v>
       </c>
@@ -10000,7 +10000,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>675</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>677</v>
       </c>
@@ -10046,7 +10046,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>548</v>
       </c>
@@ -10069,7 +10069,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>679</v>
       </c>
@@ -10092,7 +10092,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>556</v>
       </c>
@@ -10115,7 +10115,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>560</v>
       </c>
@@ -10138,7 +10138,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>680</v>
       </c>
@@ -10161,7 +10161,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>682</v>
       </c>
@@ -10184,7 +10184,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>572</v>
       </c>
@@ -10207,7 +10207,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>683</v>
       </c>
@@ -10243,18 +10243,18 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="72.83203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="72.77734375" style="5" customWidth="1"/>
     <col min="7" max="7" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -10277,7 +10277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>685</v>
       </c>
@@ -10300,7 +10300,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>689</v>
       </c>
@@ -10323,7 +10323,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>693</v>
       </c>
@@ -10346,7 +10346,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>389</v>
       </c>
@@ -10369,7 +10369,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>698</v>
       </c>
@@ -10392,7 +10392,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>702</v>
       </c>
@@ -10415,7 +10415,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="64.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>706</v>
       </c>
@@ -10438,7 +10438,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>710</v>
       </c>
@@ -10461,7 +10461,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>713</v>
       </c>
@@ -10484,7 +10484,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>717</v>
       </c>
@@ -10507,7 +10507,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>721</v>
       </c>
@@ -10530,7 +10530,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>724</v>
       </c>
@@ -10553,7 +10553,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>728</v>
       </c>
@@ -10576,7 +10576,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>731</v>
       </c>
@@ -10599,7 +10599,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>735</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>738</v>
       </c>
@@ -10645,7 +10645,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>552</v>
       </c>
@@ -10668,7 +10668,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="64.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>744</v>
       </c>
@@ -10691,7 +10691,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>748</v>
       </c>
@@ -10714,7 +10714,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>750</v>
       </c>
@@ -10737,7 +10737,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>753</v>
       </c>
@@ -10760,7 +10760,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>756</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>759</v>
       </c>
@@ -10806,7 +10806,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>762</v>
       </c>
@@ -10829,7 +10829,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -10852,7 +10852,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>766</v>
       </c>
@@ -10875,7 +10875,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -10898,7 +10898,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -10921,7 +10921,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -10944,7 +10944,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>767</v>
       </c>
@@ -10967,7 +10967,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>770</v>
       </c>
@@ -10990,7 +10990,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>772</v>
       </c>
@@ -11013,7 +11013,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>773</v>
       </c>
@@ -11036,7 +11036,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -11059,7 +11059,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>774</v>
       </c>
@@ -11082,7 +11082,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>777</v>
       </c>
@@ -11105,7 +11105,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>781</v>
       </c>
@@ -11128,7 +11128,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>785</v>
       </c>
@@ -11151,7 +11151,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>789</v>
       </c>
@@ -11174,7 +11174,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>793</v>
       </c>
@@ -11210,13 +11210,13 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="73" customWidth="1"/>
-    <col min="7" max="7" width="36.83203125" customWidth="1"/>
+    <col min="7" max="7" width="36.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -11239,7 +11239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>2</v>
       </c>
@@ -11256,7 +11256,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>5</v>
       </c>
@@ -11273,7 +11273,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -11290,7 +11290,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -11307,7 +11307,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
@@ -11324,7 +11324,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -11341,7 +11341,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1</v>
       </c>
@@ -11358,7 +11358,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1</v>
       </c>
@@ -11375,7 +11375,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1</v>
       </c>
@@ -11392,7 +11392,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>83</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>2</v>
       </c>
@@ -11426,7 +11426,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>
@@ -11443,7 +11443,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>6</v>
       </c>
@@ -11460,7 +11460,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>6</v>
       </c>
@@ -11477,7 +11477,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>2</v>
       </c>
@@ -11494,7 +11494,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>2</v>
       </c>
@@ -11511,7 +11511,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>35</v>
       </c>
@@ -11528,7 +11528,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>1</v>
       </c>
@@ -11545,7 +11545,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>1</v>
       </c>
@@ -11562,7 +11562,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>1</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>1</v>
       </c>
@@ -11596,7 +11596,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>7</v>
       </c>
@@ -11613,7 +11613,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>3</v>
       </c>
@@ -11630,7 +11630,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>4</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>2</v>
       </c>
@@ -11664,7 +11664,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>3</v>
       </c>
@@ -11681,7 +11681,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>2</v>
       </c>
@@ -11698,7 +11698,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>3</v>
       </c>
@@ -11715,7 +11715,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>2</v>
       </c>
@@ -11732,7 +11732,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>5</v>
       </c>
@@ -11749,7 +11749,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>1</v>
       </c>
@@ -11766,7 +11766,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>1</v>
       </c>
@@ -11783,7 +11783,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>10</v>
       </c>
@@ -11800,7 +11800,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>2</v>
       </c>
@@ -11817,7 +11817,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>2</v>
       </c>
@@ -11834,7 +11834,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>1</v>
       </c>
@@ -11851,7 +11851,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
idk just trying something
</commit_message>
<xml_diff>
--- a/double-major-optimization-main/Data/Sheets/Buckets.xlsx
+++ b/double-major-optimization-main/Data/Sheets/Buckets.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferkimball/WPI-Student-Course-Optimization-23-24/double-major-optimization-main/Data/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EA920F-A8BD-A041-A879-FB7BAC42C78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355C7C2B-ECDF-CA4D-8196-D35DC68CADD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN_ED" sheetId="1" r:id="rId1"/>
@@ -1924,9 +1924,6 @@
     <t>['CS_568', 'SEME_568']</t>
   </si>
   <si>
-    <t>['C_REST_G_AI_AET']</t>
-  </si>
-  <si>
     <t>HUA_DPE</t>
   </si>
   <si>
@@ -2915,6 +2912,9 @@
   </si>
   <si>
     <t>Systems or Networks: CS_502, CS_513, CS_528, CS_529, CS_533, CS_588, ECE_581, CS_535, CS_577, ECE_537</t>
+  </si>
+  <si>
+    <t>['DS_M_TOTAL_CREDITS', 'C_REST_G_AI_AET']</t>
   </si>
 </sst>
 </file>
@@ -3150,7 +3150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3221,6 +3221,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3879,7 +3882,7 @@
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -3971,19 +3974,19 @@
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>769</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
         <v>770</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>771</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>360</v>
@@ -3994,7 +3997,7 @@
     </row>
     <row r="8" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -4017,7 +4020,7 @@
     </row>
     <row r="9" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -4063,7 +4066,7 @@
     </row>
     <row r="11" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B11">
         <v>24</v>
@@ -4075,10 +4078,10 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>372</v>
@@ -4086,7 +4089,7 @@
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -4098,18 +4101,18 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
+        <v>809</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>810</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="21" t="s">
         <v>811</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -4121,64 +4124,64 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
+        <v>813</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="21" t="s">
         <v>815</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>816</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
         <v>817</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" s="5" t="s">
         <v>818</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="21" t="s">
         <v>819</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>820</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
         <v>821</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="21" t="s">
         <v>823</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -4190,18 +4193,18 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
+        <v>824</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="21" t="s">
         <v>826</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -4213,41 +4216,41 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
+        <v>828</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>829</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="21" t="s">
         <v>830</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>831</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
         <v>832</v>
       </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" s="5" t="s">
         <v>833</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="21" t="s">
         <v>834</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -4259,87 +4262,87 @@
         <v>3</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>837</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="21" t="s">
         <v>838</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>839</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
         <v>840</v>
       </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" s="5" t="s">
         <v>841</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="21" t="s">
         <v>842</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>843</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
         <v>844</v>
       </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="G21" s="21" t="s">
         <v>846</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>847</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
         <v>848</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="21" t="s">
         <v>850</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -4351,41 +4354,41 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
+        <v>852</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="21" t="s">
         <v>854</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>855</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
         <v>856</v>
       </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F24" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="21" t="s">
         <v>858</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -4397,18 +4400,18 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
+        <v>860</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="21" t="s">
         <v>862</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4420,18 +4423,18 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
+        <v>864</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>865</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="21" t="s">
         <v>866</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B27">
         <v>27</v>
@@ -4443,36 +4446,36 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F27" s="5" t="s">
+        <v>867</v>
+      </c>
+      <c r="G27" s="21" t="s">
         <v>868</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>869</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
         <v>870</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <v>3</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="21" t="s">
         <v>872</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>873</v>
       </c>
     </row>
   </sheetData>
@@ -4516,7 +4519,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -4528,12 +4531,12 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4545,12 +4548,12 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -4562,12 +4565,12 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -4579,12 +4582,12 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -4601,7 +4604,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -4613,12 +4616,12 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -4630,29 +4633,29 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
         <v>880</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -4669,7 +4672,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -4681,12 +4684,12 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -4703,7 +4706,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -4715,12 +4718,12 @@
         <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C14">
         <v>63</v>
@@ -4732,46 +4735,46 @@
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
+        <v>886</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
         <v>887</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="G15" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
+        <v>888</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
         <v>889</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -4788,7 +4791,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C18">
         <v>9</v>
@@ -4800,29 +4803,29 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
+        <v>892</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
         <v>893</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="G19" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C20">
         <v>13</v>
@@ -4834,12 +4837,12 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -4851,12 +4854,12 @@
         <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -4868,12 +4871,12 @@
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C23">
         <v>6</v>
@@ -4885,12 +4888,12 @@
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -4902,12 +4905,12 @@
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -4924,7 +4927,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -4936,12 +4939,12 @@
         <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -4958,7 +4961,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -4970,12 +4973,12 @@
         <v>3</v>
       </c>
       <c r="G28" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -4992,7 +4995,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C30">
         <v>16</v>
@@ -5004,12 +5007,12 @@
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -5021,12 +5024,12 @@
         <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -5043,7 +5046,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -5055,12 +5058,12 @@
         <v>3</v>
       </c>
       <c r="G33" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -5072,12 +5075,12 @@
         <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -5089,12 +5092,12 @@
         <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -5106,12 +5109,12 @@
         <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C37">
         <v>6</v>
@@ -5123,12 +5126,12 @@
         <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -5140,7 +5143,7 @@
         <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -5332,7 +5335,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="23" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -5344,7 +5347,7 @@
         <v>3</v>
       </c>
       <c r="G50" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -5361,7 +5364,7 @@
         <v>3</v>
       </c>
       <c r="G51" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -5395,7 +5398,7 @@
         <v>3</v>
       </c>
       <c r="G53" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -5434,7 +5437,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C56">
         <v>4</v>
@@ -5446,7 +5449,7 @@
         <v>3</v>
       </c>
       <c r="G56" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -5497,7 +5500,7 @@
         <v>3</v>
       </c>
       <c r="G59" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -5514,7 +5517,7 @@
         <v>3</v>
       </c>
       <c r="G60" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -5531,12 +5534,12 @@
         <v>3</v>
       </c>
       <c r="G61" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="23" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -5548,12 +5551,12 @@
         <v>3</v>
       </c>
       <c r="G62" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="23" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -5565,12 +5568,12 @@
         <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C64">
         <v>2</v>
@@ -5582,12 +5585,12 @@
         <v>3</v>
       </c>
       <c r="G64" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="23" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -5611,7 +5614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -5651,7 +5654,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B2">
         <v>48</v>
@@ -5663,18 +5666,18 @@
         <v>4.5</v>
       </c>
       <c r="E2" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -5686,18 +5689,18 @@
         <v>4.5</v>
       </c>
       <c r="E3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -5709,13 +5712,13 @@
         <v>4.5</v>
       </c>
       <c r="E4" t="s">
+        <v>927</v>
+      </c>
+      <c r="F4" t="s">
         <v>928</v>
       </c>
-      <c r="F4" t="s">
-        <v>929</v>
-      </c>
       <c r="G4" s="25" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -5732,18 +5735,18 @@
         <v>4.5</v>
       </c>
       <c r="E5" t="s">
+        <v>929</v>
+      </c>
+      <c r="F5" t="s">
         <v>930</v>
       </c>
-      <c r="F5" t="s">
-        <v>931</v>
-      </c>
       <c r="G5" s="25" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -5755,18 +5758,18 @@
         <v>4.5</v>
       </c>
       <c r="E6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -5781,15 +5784,15 @@
         <v>277</v>
       </c>
       <c r="F7" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5801,18 +5804,18 @@
         <v>4.5</v>
       </c>
       <c r="E8" t="s">
+        <v>932</v>
+      </c>
+      <c r="F8" t="s">
         <v>933</v>
       </c>
-      <c r="F8" t="s">
-        <v>934</v>
-      </c>
       <c r="G8" s="25" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5824,13 +5827,13 @@
         <v>13.5</v>
       </c>
       <c r="E9" t="s">
+        <v>934</v>
+      </c>
+      <c r="F9" t="s">
         <v>935</v>
       </c>
-      <c r="F9" t="s">
-        <v>936</v>
-      </c>
       <c r="G9" s="25" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
   </sheetData>
@@ -9086,8 +9089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10911,8 +10914,8 @@
       <c r="F79" t="s">
         <v>625</v>
       </c>
-      <c r="G79" s="15" t="s">
-        <v>626</v>
+      <c r="G79" s="26" t="s">
+        <v>956</v>
       </c>
     </row>
   </sheetData>
@@ -11076,7 +11079,7 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -11215,7 +11218,7 @@
     </row>
     <row r="13" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -11250,7 +11253,7 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F14" t="s">
         <v>379</v>
@@ -11261,7 +11264,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B15">
         <v>17</v>
@@ -11273,7 +11276,7 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F15" t="s">
         <v>383</v>
@@ -11284,7 +11287,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -11296,7 +11299,7 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F16" t="s">
         <v>387</v>
@@ -11307,7 +11310,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -11330,7 +11333,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -11348,12 +11351,12 @@
         <v>394</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -11365,10 +11368,10 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
+        <v>637</v>
+      </c>
+      <c r="F19" t="s">
         <v>638</v>
-      </c>
-      <c r="F19" t="s">
-        <v>639</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>403</v>
@@ -11376,7 +11379,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B20">
         <v>11</v>
@@ -11388,10 +11391,10 @@
         <v>4.5</v>
       </c>
       <c r="E20" t="s">
+        <v>640</v>
+      </c>
+      <c r="F20" t="s">
         <v>641</v>
-      </c>
-      <c r="F20" t="s">
-        <v>642</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>403</v>
@@ -11399,30 +11402,30 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>642</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
         <v>643</v>
       </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>644</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" s="16" t="s">
         <v>645</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -11434,41 +11437,41 @@
         <v>4.5</v>
       </c>
       <c r="E22" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F22" t="s">
         <v>290</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>648</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
         <v>649</v>
       </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>650</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" s="16" t="s">
         <v>651</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -11480,33 +11483,33 @@
         <v>4.5</v>
       </c>
       <c r="E24" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F24" t="s">
         <v>478</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>654</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
         <v>655</v>
       </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>656</v>
-      </c>
-      <c r="F25" t="s">
-        <v>657</v>
       </c>
       <c r="G25" s="16" t="s">
         <v>467</v>
@@ -11514,7 +11517,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -11526,10 +11529,10 @@
         <v>4.5</v>
       </c>
       <c r="E26" t="s">
+        <v>658</v>
+      </c>
+      <c r="F26" t="s">
         <v>659</v>
-      </c>
-      <c r="F26" t="s">
-        <v>660</v>
       </c>
       <c r="G26" s="16" t="s">
         <v>467</v>
@@ -11537,7 +11540,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B27">
         <v>11</v>
@@ -11549,10 +11552,10 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
+        <v>661</v>
+      </c>
+      <c r="F27" t="s">
         <v>662</v>
-      </c>
-      <c r="F27" t="s">
-        <v>663</v>
       </c>
       <c r="G27" s="16" t="s">
         <v>439</v>
@@ -11560,7 +11563,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -11572,10 +11575,10 @@
         <v>4.5</v>
       </c>
       <c r="E28" t="s">
+        <v>664</v>
+      </c>
+      <c r="F28" t="s">
         <v>665</v>
-      </c>
-      <c r="F28" t="s">
-        <v>666</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>439</v>
@@ -11583,7 +11586,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -11629,30 +11632,30 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>667</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
         <v>668</v>
       </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>669</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" s="16" t="s">
         <v>670</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -11664,18 +11667,18 @@
         <v>4.5</v>
       </c>
       <c r="E32" t="s">
+        <v>672</v>
+      </c>
+      <c r="F32" t="s">
         <v>673</v>
       </c>
-      <c r="F32" t="s">
-        <v>674</v>
-      </c>
       <c r="G32" s="16" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -11687,7 +11690,7 @@
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F33" t="s">
         <v>538</v>
@@ -11698,7 +11701,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B34">
         <v>6</v>
@@ -11710,7 +11713,7 @@
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F34" t="s">
         <v>546</v>
@@ -11744,7 +11747,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -11813,7 +11816,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B39">
         <v>150</v>
@@ -11825,7 +11828,7 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F39" t="s">
         <v>566</v>
@@ -11836,7 +11839,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -11882,19 +11885,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>682</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
         <v>683</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>3</v>
-      </c>
-      <c r="E42" t="s">
-        <v>684</v>
       </c>
       <c r="F42" t="s">
         <v>621</v>
@@ -11952,7 +11955,7 @@
     </row>
     <row r="2" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -11964,41 +11967,41 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>685</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="18" t="s">
         <v>687</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>688</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>689</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="5" t="s">
         <v>690</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="18" t="s">
         <v>691</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -12010,13 +12013,13 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
+        <v>693</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="18" t="s">
         <v>695</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12039,12 +12042,12 @@
         <v>390</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -12056,18 +12059,18 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
+        <v>698</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>699</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="18" t="s">
         <v>700</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -12079,18 +12082,18 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
+        <v>702</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>703</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="18" t="s">
         <v>704</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B8">
         <v>26</v>
@@ -12102,18 +12105,18 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
+        <v>706</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="18" t="s">
         <v>708</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B9">
         <v>57</v>
@@ -12125,41 +12128,41 @@
         <v>4.5</v>
       </c>
       <c r="E9" t="s">
+        <v>710</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>711</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>712</v>
-      </c>
       <c r="G9" s="18" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>712</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
         <v>713</v>
       </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="18" t="s">
         <v>715</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -12171,18 +12174,18 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
+        <v>717</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>718</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="18" t="s">
         <v>719</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -12194,18 +12197,18 @@
         <v>4.5</v>
       </c>
       <c r="E12" t="s">
+        <v>721</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>723</v>
-      </c>
       <c r="G12" s="18" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -12217,18 +12220,18 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
+        <v>724</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>725</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="18" t="s">
         <v>726</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -12240,18 +12243,18 @@
         <v>4.5</v>
       </c>
       <c r="E14" t="s">
+        <v>728</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>729</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>730</v>
-      </c>
       <c r="G14" s="18" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -12263,18 +12266,18 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
+        <v>731</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="18" t="s">
         <v>733</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -12286,36 +12289,36 @@
         <v>4.5</v>
       </c>
       <c r="E16" t="s">
+        <v>735</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>737</v>
-      </c>
       <c r="G16" s="18" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>737</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
         <v>738</v>
       </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" s="5" t="s">
         <v>739</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="18" t="s">
         <v>740</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12332,18 +12335,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>554</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B19">
         <v>29</v>
@@ -12355,18 +12358,18 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
+        <v>744</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>745</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="18" t="s">
         <v>746</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -12378,18 +12381,18 @@
         <v>4.5</v>
       </c>
       <c r="E20" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -12401,18 +12404,18 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
+        <v>749</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>750</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="G21" s="18" t="s">
         <v>751</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -12424,18 +12427,18 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
+        <v>752</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>753</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="18" t="s">
         <v>754</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B23">
         <v>10</v>
@@ -12447,18 +12450,18 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
+        <v>755</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>756</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="18" t="s">
         <v>757</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -12470,18 +12473,18 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
+        <v>758</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>759</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="18" t="s">
         <v>760</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B25">
         <v>20</v>
@@ -12493,13 +12496,13 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
+        <v>762</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>763</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="18" t="s">
         <v>764</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12527,7 +12530,7 @@
     </row>
     <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -12619,42 +12622,42 @@
     </row>
     <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>766</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
         <v>767</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31" t="s">
-        <v>768</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>357</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>769</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
         <v>770</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32">
-        <v>3</v>
-      </c>
-      <c r="E32" t="s">
-        <v>771</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>360</v>
@@ -12665,7 +12668,7 @@
     </row>
     <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -12688,7 +12691,7 @@
     </row>
     <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -12734,7 +12737,7 @@
     </row>
     <row r="36" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B36">
         <v>10</v>
@@ -12746,10 +12749,10 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
+        <v>774</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>775</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>776</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>372</v>
@@ -12757,53 +12760,53 @@
     </row>
     <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>776</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
         <v>777</v>
       </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
-        <v>3</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="F37" s="5" t="s">
         <v>778</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="G37" s="18" t="s">
         <v>779</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>780</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
         <v>781</v>
       </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="D38">
-        <v>3</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="F38" s="5" t="s">
         <v>782</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="G38" s="18" t="s">
         <v>783</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -12815,18 +12818,18 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
+        <v>785</v>
+      </c>
+      <c r="F39" t="s">
         <v>786</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" s="20" t="s">
         <v>787</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -12838,18 +12841,18 @@
         <v>3</v>
       </c>
       <c r="E40" t="s">
+        <v>789</v>
+      </c>
+      <c r="F40" t="s">
         <v>790</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" s="20" t="s">
         <v>791</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -12861,13 +12864,13 @@
         <v>3</v>
       </c>
       <c r="E41" t="s">
+        <v>793</v>
+      </c>
+      <c r="F41" t="s">
         <v>794</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" s="20" t="s">
         <v>795</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>796</v>
       </c>
     </row>
   </sheetData>
@@ -12923,10 +12926,10 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>787</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -12940,10 +12943,10 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -12957,10 +12960,10 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
+        <v>690</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>691</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -12974,10 +12977,10 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
+        <v>790</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>791</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -12991,10 +12994,10 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
+        <v>794</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>795</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -13008,10 +13011,10 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
+        <v>694</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>695</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -13028,7 +13031,7 @@
         <v>390</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -13042,10 +13045,10 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
+        <v>699</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>700</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -13059,10 +13062,10 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -13076,10 +13079,10 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -13093,10 +13096,10 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>715</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -13110,10 +13113,10 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -13127,10 +13130,10 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -13144,10 +13147,10 @@
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -13161,10 +13164,10 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
+        <v>739</v>
+      </c>
+      <c r="G16" s="20" t="s">
         <v>740</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
@@ -13181,7 +13184,7 @@
         <v>554</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
@@ -13195,10 +13198,10 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -13212,10 +13215,10 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
+        <v>750</v>
+      </c>
+      <c r="G19" s="20" t="s">
         <v>751</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
@@ -13229,10 +13232,10 @@
         <v>3</v>
       </c>
       <c r="F20" t="s">
+        <v>753</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>754</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
@@ -13246,10 +13249,10 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
+        <v>756</v>
+      </c>
+      <c r="G21" s="20" t="s">
         <v>757</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
@@ -13263,10 +13266,10 @@
         <v>3</v>
       </c>
       <c r="F22" t="s">
+        <v>759</v>
+      </c>
+      <c r="G22" s="20" t="s">
         <v>760</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -13280,10 +13283,10 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
+        <v>763</v>
+      </c>
+      <c r="G23" s="20" t="s">
         <v>764</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -13385,7 +13388,7 @@
         <v>357</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -13467,7 +13470,7 @@
         <v>3</v>
       </c>
       <c r="F34" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>372</v>
@@ -13484,10 +13487,10 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
+        <v>778</v>
+      </c>
+      <c r="G35" s="20" t="s">
         <v>779</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -13501,10 +13504,10 @@
         <v>3</v>
       </c>
       <c r="F36" t="s">
+        <v>803</v>
+      </c>
+      <c r="G36" s="20" t="s">
         <v>804</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -13518,10 +13521,10 @@
         <v>3</v>
       </c>
       <c r="F37" t="s">
+        <v>805</v>
+      </c>
+      <c r="G37" s="20" t="s">
         <v>806</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -13535,10 +13538,10 @@
         <v>3</v>
       </c>
       <c r="F38" t="s">
+        <v>782</v>
+      </c>
+      <c r="G38" s="20" t="s">
         <v>783</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did this work now?
</commit_message>
<xml_diff>
--- a/double-major-optimization-main/Data/Sheets/Buckets.xlsx
+++ b/double-major-optimization-main/Data/Sheets/Buckets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferkimball/WPI-Student-Course-Optimization-23-24/double-major-optimization-main/Data/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C546001-5291-6D41-893C-234DACB1720C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158B91A1-D73B-4F40-823B-6C0F23890F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="1106">
   <si>
     <t>Bucket Key</t>
   </si>
@@ -1928,6 +1928,9 @@
     <t>MA_ELECT</t>
   </si>
   <si>
+    <t>Math Disciplinary Electives</t>
+  </si>
+  <si>
     <t>CS_ELECT</t>
   </si>
   <si>
@@ -3348,12 +3351,6 @@
   </si>
   <si>
     <t>['BME_520', 'RBE_520', 'BME_523', 'BME_330', 'ME_5359', 'MTE_559', 'BME_531', 'BME_532', 'BME_533', 'ME_5503', 'BME_535', 'BME_553', 'BME_555', 'BME_560', 'BME_562', 'BME_564', 'BME_580', 'RBE_580', 'ME_5205', 'BME_581', 'BME_583', 'BME_591', 'BME_592', 'BME_593', 'BME_594', 'BME_595', 'BME_596', 'BME_597', 'BME_598', 'BME_599', 'BME_698']</t>
-  </si>
-  <si>
-    <t>Systems - CS_3013, CS_4513, CS_4515, CS_4516</t>
-  </si>
-  <si>
-    <t>Disciplinary Electives</t>
   </si>
 </sst>
 </file>
@@ -4376,7 +4373,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B2">
         <v>48</v>
@@ -4388,18 +4385,18 @@
         <v>4.5</v>
       </c>
       <c r="E2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="F2" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -4411,18 +4408,18 @@
         <v>4.5</v>
       </c>
       <c r="E3" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="F3" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -4434,13 +4431,13 @@
         <v>4.5</v>
       </c>
       <c r="E4" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="F4" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4457,18 +4454,18 @@
         <v>4.5</v>
       </c>
       <c r="E5" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F5" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -4480,18 +4477,18 @@
         <v>4.5</v>
       </c>
       <c r="E6" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="F6" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -4506,15 +4503,15 @@
         <v>277</v>
       </c>
       <c r="F7" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4526,18 +4523,18 @@
         <v>4.5</v>
       </c>
       <c r="E8" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="F8" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4549,13 +4546,13 @@
         <v>13.5</v>
       </c>
       <c r="E9" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="F9" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>
@@ -4630,7 +4627,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -4722,7 +4719,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -4740,12 +4737,12 @@
         <v>357</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -4757,7 +4754,7 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F8" t="s">
         <v>360</v>
@@ -4768,7 +4765,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -4780,7 +4777,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="F9" t="s">
         <v>363</v>
@@ -4791,7 +4788,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4803,7 +4800,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="F10" t="s">
         <v>366</v>
@@ -4837,7 +4834,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B12">
         <v>12</v>
@@ -4852,7 +4849,7 @@
         <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="G12" s="26" t="s">
         <v>372</v>
@@ -4860,7 +4857,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B13">
         <v>53</v>
@@ -4872,18 +4869,18 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="F13" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -4895,18 +4892,18 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="F14" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -4918,18 +4915,18 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="F15" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -4941,18 +4938,18 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="F16" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B17">
         <v>28</v>
@@ -4964,18 +4961,18 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="F17" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -4987,18 +4984,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="F18" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B19">
         <v>77</v>
@@ -5010,18 +5007,18 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="F19" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -5033,18 +5030,18 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="F20" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -5056,18 +5053,18 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="F21" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -5079,18 +5076,18 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="F22" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -5102,18 +5099,18 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="F23" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5125,18 +5122,18 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="F24" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B25">
         <v>42</v>
@@ -5148,18 +5145,18 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="F25" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B26">
         <v>158</v>
@@ -5171,13 +5168,13 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="F26" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
   </sheetData>
@@ -5252,7 +5249,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -5344,7 +5341,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -5356,18 +5353,18 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="F7" t="s">
         <v>357</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -5379,7 +5376,7 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F8" t="s">
         <v>360</v>
@@ -5390,7 +5387,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -5402,7 +5399,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="F9" t="s">
         <v>363</v>
@@ -5413,7 +5410,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5425,7 +5422,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="F10" t="s">
         <v>366</v>
@@ -5459,7 +5456,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B12">
         <v>12</v>
@@ -5474,7 +5471,7 @@
         <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="G12" s="27" t="s">
         <v>372</v>
@@ -5482,7 +5479,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5494,18 +5491,18 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="F13" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -5517,18 +5514,18 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="F14" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -5540,18 +5537,18 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="F15" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B16">
         <v>156</v>
@@ -5563,18 +5560,18 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="F16" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -5586,18 +5583,18 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="F17" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -5609,18 +5606,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="F18" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -5632,18 +5629,18 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="F19" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -5655,18 +5652,18 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="F20" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -5678,18 +5675,18 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="F21" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -5701,18 +5698,18 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="F22" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -5724,18 +5721,18 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="F23" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5747,18 +5744,18 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="F24" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B25">
         <v>31</v>
@@ -5770,18 +5767,18 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="F25" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -5793,18 +5790,18 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="F26" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -5816,18 +5813,18 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="F27" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -5839,18 +5836,18 @@
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="F28" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B29">
         <v>140</v>
@@ -5862,18 +5859,18 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="F29" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -5885,13 +5882,13 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="F30" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
   </sheetData>
@@ -5903,8 +5900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5943,7 +5940,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -5955,18 +5952,18 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="F2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -5978,18 +5975,18 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="F3" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -6001,18 +5998,18 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="F4" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -6024,18 +6021,18 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="F5" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -6047,41 +6044,41 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="F6" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>1105</v>
+        <v>694</v>
       </c>
       <c r="F7" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -6093,18 +6090,18 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="F8" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6122,15 +6119,15 @@
         <v>390</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>99</v>
@@ -6139,18 +6136,18 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F10" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B11">
         <v>79</v>
@@ -6162,18 +6159,18 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="F11" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -6188,15 +6185,15 @@
         <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -6208,18 +6205,18 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="F13" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -6231,18 +6228,18 @@
         <v>4.5</v>
       </c>
       <c r="E14" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="F14" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -6254,18 +6251,18 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="F15" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -6277,18 +6274,18 @@
         <v>4.5</v>
       </c>
       <c r="E16" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="F16" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -6300,18 +6297,18 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="F17" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -6323,18 +6320,18 @@
         <v>4.5</v>
       </c>
       <c r="E18" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="F18" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -6346,18 +6343,18 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="F19" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -6369,13 +6366,13 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="F20" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -6392,18 +6389,18 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="F21" t="s">
         <v>554</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -6415,18 +6412,18 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="F22" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B23">
         <v>49</v>
@@ -6438,18 +6435,18 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="F23" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B24">
         <v>47</v>
@@ -6461,18 +6458,18 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="F24" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -6484,18 +6481,18 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="F25" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B26">
         <v>26</v>
@@ -6507,18 +6504,18 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="F26" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -6530,18 +6527,18 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="F27" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B28">
         <v>29</v>
@@ -6553,13 +6550,13 @@
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="F28" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -6576,13 +6573,13 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="F29" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -6599,13 +6596,13 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="F30" t="s">
         <v>621</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -6633,7 +6630,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B32">
         <v>20</v>
@@ -6725,7 +6722,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -6737,18 +6734,18 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="F36" t="s">
         <v>357</v>
       </c>
       <c r="G36" s="28" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -6760,7 +6757,7 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F37" t="s">
         <v>360</v>
@@ -6771,7 +6768,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B38">
         <v>100</v>
@@ -6783,7 +6780,7 @@
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="F38" t="s">
         <v>363</v>
@@ -6794,7 +6791,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -6806,7 +6803,7 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="F39" t="s">
         <v>366</v>
@@ -6840,7 +6837,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B41">
         <v>10</v>
@@ -6855,7 +6852,7 @@
         <v>36</v>
       </c>
       <c r="F41" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="G41" s="28" t="s">
         <v>372</v>
@@ -6863,7 +6860,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -6875,18 +6872,18 @@
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="F42" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -6898,18 +6895,18 @@
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="F43" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="G43" s="28" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -6921,13 +6918,13 @@
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F44" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="G44" s="28" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>
@@ -7076,7 +7073,7 @@
         <v>357</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7158,7 +7155,7 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="G12" s="30" t="s">
         <v>372</v>
@@ -7175,10 +7172,10 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G13" s="30" t="s">
         <v>1047</v>
-      </c>
-      <c r="G13" s="30" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -7192,10 +7189,10 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
+        <v>1050</v>
+      </c>
+      <c r="G14" s="30" t="s">
         <v>1049</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -7209,10 +7206,10 @@
         <v>3</v>
       </c>
       <c r="F15" t="s">
+        <v>1052</v>
+      </c>
+      <c r="G15" s="30" t="s">
         <v>1051</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -7226,10 +7223,10 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
@@ -7243,10 +7240,10 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
@@ -7260,10 +7257,10 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -7277,10 +7274,10 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G19" s="30" t="s">
         <v>1056</v>
-      </c>
-      <c r="G19" s="30" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
@@ -7294,10 +7291,10 @@
         <v>3</v>
       </c>
       <c r="F20" t="s">
+        <v>1059</v>
+      </c>
+      <c r="G20" s="30" t="s">
         <v>1058</v>
-      </c>
-      <c r="G20" s="30" t="s">
-        <v>1057</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
@@ -7311,10 +7308,10 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
@@ -7328,10 +7325,10 @@
         <v>3</v>
       </c>
       <c r="F22" t="s">
+        <v>1062</v>
+      </c>
+      <c r="G22" s="30" t="s">
         <v>1061</v>
-      </c>
-      <c r="G22" s="30" t="s">
-        <v>1060</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -7345,10 +7342,10 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G23" s="30" t="s">
         <v>1063</v>
-      </c>
-      <c r="G23" s="30" t="s">
-        <v>1062</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -7362,10 +7359,10 @@
         <v>3</v>
       </c>
       <c r="F24" t="s">
+        <v>1066</v>
+      </c>
+      <c r="G24" s="30" t="s">
         <v>1065</v>
-      </c>
-      <c r="G24" s="30" t="s">
-        <v>1064</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
@@ -7379,10 +7376,10 @@
         <v>3</v>
       </c>
       <c r="F25" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G25" s="30" t="s">
         <v>1067</v>
-      </c>
-      <c r="G25" s="30" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -7396,10 +7393,10 @@
         <v>3</v>
       </c>
       <c r="F26" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G26" s="30" t="s">
         <v>1069</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>1068</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
@@ -7413,10 +7410,10 @@
         <v>3</v>
       </c>
       <c r="F27" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G27" s="30" t="s">
         <v>1071</v>
-      </c>
-      <c r="G27" s="30" t="s">
-        <v>1070</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
@@ -7430,10 +7427,10 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
+        <v>1074</v>
+      </c>
+      <c r="G28" s="30" t="s">
         <v>1073</v>
-      </c>
-      <c r="G28" s="30" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
@@ -7447,10 +7444,10 @@
         <v>3</v>
       </c>
       <c r="F29" t="s">
+        <v>1076</v>
+      </c>
+      <c r="G29" s="30" t="s">
         <v>1075</v>
-      </c>
-      <c r="G29" s="30" t="s">
-        <v>1074</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -7464,10 +7461,10 @@
         <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
@@ -7481,10 +7478,10 @@
         <v>3</v>
       </c>
       <c r="F31" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G31" s="30" t="s">
         <v>1078</v>
-      </c>
-      <c r="G31" s="30" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
@@ -7498,10 +7495,10 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G32" s="30" t="s">
         <v>1080</v>
-      </c>
-      <c r="G32" s="30" t="s">
-        <v>1079</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
@@ -7515,10 +7512,10 @@
         <v>3</v>
       </c>
       <c r="F33" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G33" s="30" t="s">
         <v>1082</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>1081</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
@@ -7532,10 +7529,10 @@
         <v>3</v>
       </c>
       <c r="F34" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G34" s="30" t="s">
         <v>1084</v>
-      </c>
-      <c r="G34" s="30" t="s">
-        <v>1083</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
@@ -7549,10 +7546,10 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G35" s="30" t="s">
         <v>1086</v>
-      </c>
-      <c r="G35" s="30" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -7566,10 +7563,10 @@
         <v>3</v>
       </c>
       <c r="F36" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G36" s="30" t="s">
         <v>1088</v>
-      </c>
-      <c r="G36" s="30" t="s">
-        <v>1087</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -7583,10 +7580,10 @@
         <v>3</v>
       </c>
       <c r="F37" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G37" s="30" t="s">
         <v>1090</v>
-      </c>
-      <c r="G37" s="30" t="s">
-        <v>1089</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -7600,10 +7597,10 @@
         <v>3</v>
       </c>
       <c r="F38" t="s">
+        <v>1093</v>
+      </c>
+      <c r="G38" s="30" t="s">
         <v>1092</v>
-      </c>
-      <c r="G38" s="30" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
@@ -7617,10 +7614,10 @@
         <v>3</v>
       </c>
       <c r="F39" t="s">
+        <v>1095</v>
+      </c>
+      <c r="G39" s="30" t="s">
         <v>1094</v>
-      </c>
-      <c r="G39" s="30" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
@@ -7634,10 +7631,10 @@
         <v>3</v>
       </c>
       <c r="F40" t="s">
+        <v>1097</v>
+      </c>
+      <c r="G40" s="30" t="s">
         <v>1096</v>
-      </c>
-      <c r="G40" s="30" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
@@ -7651,10 +7648,10 @@
         <v>3</v>
       </c>
       <c r="F41" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G41" s="30" t="s">
         <v>1098</v>
-      </c>
-      <c r="G41" s="30" t="s">
-        <v>1097</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
@@ -7668,10 +7665,10 @@
         <v>3</v>
       </c>
       <c r="F42" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G42" s="30" t="s">
         <v>1100</v>
-      </c>
-      <c r="G42" s="30" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
@@ -7685,10 +7682,10 @@
         <v>3</v>
       </c>
       <c r="F43" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G43" s="30" t="s">
         <v>1102</v>
-      </c>
-      <c r="G43" s="30" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
@@ -7702,10 +7699,10 @@
         <v>3</v>
       </c>
       <c r="F44" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G44" s="30" t="s">
         <v>1104</v>
-      </c>
-      <c r="G44" s="30" t="s">
-        <v>1103</v>
       </c>
     </row>
   </sheetData>
@@ -12799,8 +12796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13151,7 +13148,7 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>1106</v>
+        <v>631</v>
       </c>
       <c r="F15" t="s">
         <v>383</v>
@@ -13162,7 +13159,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -13174,7 +13171,7 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F16" t="s">
         <v>387</v>
@@ -13185,7 +13182,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -13208,7 +13205,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -13226,12 +13223,12 @@
         <v>394</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -13243,10 +13240,10 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F19" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>403</v>
@@ -13254,7 +13251,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B20">
         <v>11</v>
@@ -13266,10 +13263,10 @@
         <v>4.5</v>
       </c>
       <c r="E20" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="F20" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>403</v>
@@ -13277,7 +13274,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -13289,18 +13286,18 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="F21" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -13312,18 +13309,18 @@
         <v>4.5</v>
       </c>
       <c r="E22" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F22" t="s">
         <v>290</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -13335,18 +13332,18 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F23" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -13358,18 +13355,18 @@
         <v>4.5</v>
       </c>
       <c r="E24" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="F24" t="s">
         <v>478</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -13381,10 +13378,10 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="F25" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="G25" s="16" t="s">
         <v>467</v>
@@ -13392,7 +13389,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -13404,10 +13401,10 @@
         <v>4.5</v>
       </c>
       <c r="E26" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="F26" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G26" s="16" t="s">
         <v>467</v>
@@ -13415,7 +13412,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B27">
         <v>11</v>
@@ -13427,10 +13424,10 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="F27" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="G27" s="16" t="s">
         <v>439</v>
@@ -13438,7 +13435,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -13450,10 +13447,10 @@
         <v>4.5</v>
       </c>
       <c r="E28" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="F28" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>439</v>
@@ -13461,7 +13458,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -13507,7 +13504,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -13519,18 +13516,18 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="F31" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -13542,18 +13539,18 @@
         <v>4.5</v>
       </c>
       <c r="E32" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="F32" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -13565,7 +13562,7 @@
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F33" t="s">
         <v>538</v>
@@ -13576,7 +13573,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B34">
         <v>6</v>
@@ -13588,7 +13585,7 @@
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="F34" t="s">
         <v>546</v>
@@ -13622,7 +13619,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -13691,7 +13688,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B39">
         <v>150</v>
@@ -13703,7 +13700,7 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="F39" t="s">
         <v>566</v>
@@ -13714,7 +13711,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -13760,7 +13757,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -13772,7 +13769,7 @@
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="F42" t="s">
         <v>621</v>
@@ -13830,7 +13827,7 @@
     </row>
     <row r="2" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -13842,18 +13839,18 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13865,18 +13862,18 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -13888,13 +13885,13 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -13917,12 +13914,12 @@
         <v>390</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -13934,18 +13931,18 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -13957,18 +13954,18 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B8">
         <v>26</v>
@@ -13980,18 +13977,18 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B9">
         <v>57</v>
@@ -14003,18 +14000,18 @@
         <v>4.5</v>
       </c>
       <c r="E9" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -14026,18 +14023,18 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -14049,18 +14046,18 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -14072,18 +14069,18 @@
         <v>4.5</v>
       </c>
       <c r="E12" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -14095,18 +14092,18 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -14118,18 +14115,18 @@
         <v>4.5</v>
       </c>
       <c r="E14" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -14141,18 +14138,18 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -14164,18 +14161,18 @@
         <v>4.5</v>
       </c>
       <c r="E16" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -14187,13 +14184,13 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14210,18 +14207,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>554</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B19">
         <v>29</v>
@@ -14233,18 +14230,18 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -14256,18 +14253,18 @@
         <v>4.5</v>
       </c>
       <c r="E20" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -14279,18 +14276,18 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -14302,18 +14299,18 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B23">
         <v>10</v>
@@ -14325,18 +14322,18 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -14348,18 +14345,18 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B25">
         <v>20</v>
@@ -14371,13 +14368,13 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14405,7 +14402,7 @@
     </row>
     <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -14497,7 +14494,7 @@
     </row>
     <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -14509,18 +14506,18 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>357</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -14532,7 +14529,7 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>360</v>
@@ -14543,7 +14540,7 @@
     </row>
     <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -14566,7 +14563,7 @@
     </row>
     <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -14612,7 +14609,7 @@
     </row>
     <row r="36" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B36">
         <v>10</v>
@@ -14624,10 +14621,10 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>372</v>
@@ -14635,7 +14632,7 @@
     </row>
     <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -14647,18 +14644,18 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -14670,18 +14667,18 @@
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -14693,18 +14690,18 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="F39" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -14716,18 +14713,18 @@
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="F40" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -14739,13 +14736,13 @@
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="F41" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
   </sheetData>
@@ -14817,7 +14814,7 @@
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -14909,7 +14906,7 @@
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -14921,7 +14918,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>360</v>
@@ -14932,7 +14929,7 @@
     </row>
     <row r="8" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -14955,7 +14952,7 @@
     </row>
     <row r="9" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -15001,7 +14998,7 @@
     </row>
     <row r="11" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B11">
         <v>24</v>
@@ -15013,10 +15010,10 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>372</v>
@@ -15024,7 +15021,7 @@
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -15036,18 +15033,18 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -15059,18 +15056,18 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -15082,18 +15079,18 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -15105,18 +15102,18 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -15128,18 +15125,18 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -15151,18 +15148,18 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -15174,18 +15171,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -15197,18 +15194,18 @@
         <v>3</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -15220,18 +15217,18 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -15243,18 +15240,18 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -15266,18 +15263,18 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -15289,18 +15286,18 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -15312,18 +15309,18 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -15335,18 +15332,18 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -15358,18 +15355,18 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B27">
         <v>27</v>
@@ -15381,18 +15378,18 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -15404,13 +15401,13 @@
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>